<commit_message>
Lodiang via CSV to local database
</commit_message>
<xml_diff>
--- a/data/2021-11-19 Roder связи.xlsx
+++ b/data/2021-11-19 Roder связи.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="340">
   <si>
     <t xml:space="preserve">Идентификатор операции</t>
   </si>
@@ -316,18 +316,21 @@
     <t xml:space="preserve">R1190, R1100</t>
   </si>
   <si>
+    <t xml:space="preserve">R1820, R1830, R1870, R1280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        R1850</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сборка Стойка торцевая средняя (104886)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">R1820, R1830, R1870</t>
   </si>
   <si>
-    <t xml:space="preserve">        R1850</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сборка Стойка торцевая средняя (104886)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.00</t>
-  </si>
-  <si>
     <t xml:space="preserve">        R1860</t>
   </si>
   <si>
@@ -490,7 +493,7 @@
     <t xml:space="preserve">16.00</t>
   </si>
   <si>
-    <t xml:space="preserve">R1780, R1870</t>
+    <t xml:space="preserve">R1780, R1870, R1840</t>
   </si>
   <si>
     <t xml:space="preserve">R1270</t>
@@ -518,6 +521,9 @@
   </si>
   <si>
     <t xml:space="preserve">Установка Панель алюминиевая ()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xx1230</t>
   </si>
   <si>
     <t xml:space="preserve">47.00</t>
@@ -1229,20 +1235,20 @@
   </sheetPr>
   <dimension ref="A1:N116"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A116" activeCellId="0" sqref="A116"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="87.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="73.85"/>
   </cols>
   <sheetData>
@@ -2033,18 +2039,18 @@
         <v>97</v>
       </c>
       <c r="N32" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>182249</v>
@@ -2068,24 +2074,24 @@
         <v>97</v>
       </c>
       <c r="N33" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>102031</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G34" s="0" t="s">
         <v>88</v>
@@ -2103,24 +2109,24 @@
         <v>80</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>131723</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G35" s="0" t="s">
         <v>88</v>
@@ -2138,18 +2144,18 @@
         <v>80</v>
       </c>
       <c r="N35" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H36" s="0" t="n">
         <v>0</v>
@@ -2158,27 +2164,27 @@
         <v>44545</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="N36" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>111488</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G37" s="0" t="s">
         <v>88</v>
@@ -2193,27 +2199,27 @@
         <v>44552</v>
       </c>
       <c r="M37" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N37" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>111727</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G38" s="0" t="s">
         <v>88</v>
@@ -2228,27 +2234,27 @@
         <v>44552</v>
       </c>
       <c r="M38" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N38" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>165658</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G39" s="0" t="s">
         <v>88</v>
@@ -2266,24 +2272,24 @@
         <v>100</v>
       </c>
       <c r="M39" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>100295</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G40" s="0" t="s">
         <v>88</v>
@@ -2301,15 +2307,15 @@
         <v>100</v>
       </c>
       <c r="M40" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H41" s="0" t="n">
         <v>12</v>
@@ -2323,16 +2329,16 @@
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G42" s="0" t="s">
         <v>88</v>
@@ -2350,24 +2356,24 @@
         <v>638</v>
       </c>
       <c r="M42" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N42" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G43" s="0" t="s">
         <v>88</v>
@@ -2382,24 +2388,24 @@
         <v>44540</v>
       </c>
       <c r="M43" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="N43" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G44" s="0" t="s">
         <v>88</v>
@@ -2414,18 +2420,18 @@
         <v>44547</v>
       </c>
       <c r="M44" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N44" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H45" s="0" t="n">
         <v>3</v>
@@ -2439,16 +2445,16 @@
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="F46" s="0" t="s">
         <v>146</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="F46" s="0" t="s">
-        <v>145</v>
       </c>
       <c r="G46" s="0" t="s">
         <v>88</v>
@@ -2469,15 +2475,15 @@
         <v>33</v>
       </c>
       <c r="N46" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H47" s="0" t="n">
         <v>11</v>
@@ -2491,19 +2497,19 @@
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>166069</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G48" s="0" t="s">
         <v>88</v>
@@ -2521,27 +2527,27 @@
         <v>100</v>
       </c>
       <c r="M48" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="N48" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>166069</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G49" s="0" t="s">
         <v>88</v>
@@ -2556,27 +2562,27 @@
         <v>44554</v>
       </c>
       <c r="M49" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="N49" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>118060</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G50" s="0" t="s">
         <v>88</v>
@@ -2594,24 +2600,27 @@
         <v>45</v>
       </c>
       <c r="M50" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N50" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>167</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G51" s="0" t="s">
         <v>88</v>
@@ -2629,18 +2638,18 @@
         <v>242</v>
       </c>
       <c r="M51" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="N51" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H52" s="0" t="n">
         <v>4</v>
@@ -2654,19 +2663,19 @@
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>165160</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G53" s="0" t="s">
         <v>88</v>
@@ -2684,24 +2693,24 @@
         <v>10</v>
       </c>
       <c r="M53" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N53" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G54" s="0" t="s">
         <v>88</v>
@@ -2719,15 +2728,15 @@
         <v>40</v>
       </c>
       <c r="M54" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N54" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>17</v>
@@ -2744,16 +2753,16 @@
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H56" s="0" t="n">
         <v>1</v>
@@ -2768,21 +2777,21 @@
         <v>132</v>
       </c>
       <c r="M56" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="N56" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G57" s="0" t="s">
         <v>88</v>
@@ -2800,21 +2809,21 @@
         <v>2</v>
       </c>
       <c r="M57" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="N57" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G58" s="0" t="s">
         <v>88</v>
@@ -2832,24 +2841,24 @@
         <v>4</v>
       </c>
       <c r="M58" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="N58" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H59" s="0" t="n">
         <v>3</v>
@@ -2864,21 +2873,21 @@
         <v>100</v>
       </c>
       <c r="M59" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="N59" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="G60" s="0" t="s">
         <v>88</v>
@@ -2896,21 +2905,21 @@
         <v>219</v>
       </c>
       <c r="M60" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="N60" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="G61" s="0" t="s">
         <v>88</v>
@@ -2928,21 +2937,21 @@
         <v>129</v>
       </c>
       <c r="M61" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="N61" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="G62" s="0" t="s">
         <v>88</v>
@@ -2960,21 +2969,21 @@
         <v>151</v>
       </c>
       <c r="M62" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="N62" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G63" s="0" t="s">
         <v>88</v>
@@ -2992,15 +3001,15 @@
         <v>10</v>
       </c>
       <c r="M63" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="N63" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F64" s="0" t="s">
         <v>17</v>
@@ -3017,7 +3026,7 @@
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="F65" s="0" t="s">
         <v>17</v>
@@ -3034,16 +3043,16 @@
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H66" s="0" t="n">
         <v>6</v>
@@ -3058,24 +3067,24 @@
         <v>100</v>
       </c>
       <c r="M66" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="N66" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H67" s="0" t="n">
         <v>7</v>
@@ -3090,15 +3099,15 @@
         <v>100</v>
       </c>
       <c r="M67" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="N67" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F68" s="0" t="s">
         <v>17</v>
@@ -3115,16 +3124,16 @@
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H69" s="0" t="n">
         <v>6</v>
@@ -3139,24 +3148,24 @@
         <v>100</v>
       </c>
       <c r="M69" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="N69" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="B70" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="B70" s="0" t="s">
-        <v>213</v>
-      </c>
       <c r="D70" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H70" s="0" t="n">
         <v>7</v>
@@ -3171,15 +3180,15 @@
         <v>100</v>
       </c>
       <c r="M70" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="N70" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="F71" s="0" t="s">
         <v>17</v>
@@ -3196,13 +3205,13 @@
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="G72" s="0" t="s">
         <v>88</v>
@@ -3220,24 +3229,24 @@
         <v>27</v>
       </c>
       <c r="M72" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="N72" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B73" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="B73" s="0" t="s">
-        <v>219</v>
-      </c>
       <c r="D73" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H73" s="0" t="n">
         <v>6</v>
@@ -3252,24 +3261,24 @@
         <v>100</v>
       </c>
       <c r="M73" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="N73" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H74" s="0" t="n">
         <v>7</v>
@@ -3284,15 +3293,15 @@
         <v>100</v>
       </c>
       <c r="M74" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="N74" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F75" s="0" t="s">
         <v>17</v>
@@ -3309,7 +3318,7 @@
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F76" s="0" t="s">
         <v>17</v>
@@ -3326,16 +3335,16 @@
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H77" s="0" t="n">
         <v>3</v>
@@ -3350,21 +3359,21 @@
         <v>100</v>
       </c>
       <c r="M77" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="N77" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G78" s="0" t="s">
         <v>88</v>
@@ -3382,21 +3391,21 @@
         <v>361</v>
       </c>
       <c r="M78" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="N78" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="G79" s="0" t="s">
         <v>88</v>
@@ -3414,21 +3423,21 @@
         <v>46</v>
       </c>
       <c r="M79" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="N79" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="G80" s="0" t="s">
         <v>88</v>
@@ -3446,24 +3455,24 @@
         <v>6</v>
       </c>
       <c r="M80" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="N80" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="H81" s="0" t="n">
         <v>4</v>
@@ -3478,21 +3487,21 @@
         <v>1</v>
       </c>
       <c r="M81" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="N81" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G82" s="0" t="s">
         <v>88</v>
@@ -3510,24 +3519,24 @@
         <v>4</v>
       </c>
       <c r="M82" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="N82" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H83" s="0" t="n">
         <v>3</v>
@@ -3542,15 +3551,15 @@
         <v>100</v>
       </c>
       <c r="M83" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="N83" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F84" s="0" t="s">
         <v>17</v>
@@ -3567,13 +3576,13 @@
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G85" s="0" t="s">
         <v>88</v>
@@ -3591,24 +3600,24 @@
         <v>10</v>
       </c>
       <c r="M85" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="N85" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H86" s="0" t="n">
         <v>4</v>
@@ -3623,24 +3632,24 @@
         <v>100</v>
       </c>
       <c r="M86" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="N86" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H87" s="0" t="n">
         <v>7</v>
@@ -3655,24 +3664,24 @@
         <v>100</v>
       </c>
       <c r="M87" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="N87" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="H88" s="0" t="n">
         <v>2</v>
@@ -3687,21 +3696,21 @@
         <v>2</v>
       </c>
       <c r="M88" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="N88" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="G89" s="0" t="s">
         <v>88</v>
@@ -3719,21 +3728,21 @@
         <v>1</v>
       </c>
       <c r="M89" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="N89" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="G90" s="0" t="s">
         <v>88</v>
@@ -3751,15 +3760,15 @@
         <v>13</v>
       </c>
       <c r="M90" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="N90" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="F91" s="0" t="s">
         <v>17</v>
@@ -3776,16 +3785,16 @@
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H92" s="0" t="n">
         <v>3</v>
@@ -3800,24 +3809,24 @@
         <v>100</v>
       </c>
       <c r="M92" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="N92" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H93" s="0" t="n">
         <v>3</v>
@@ -3832,24 +3841,24 @@
         <v>100</v>
       </c>
       <c r="M93" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="N93" s="0" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H94" s="0" t="n">
         <v>3</v>
@@ -3864,15 +3873,15 @@
         <v>100</v>
       </c>
       <c r="M94" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="N94" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="F95" s="0" t="s">
         <v>17</v>
@@ -3889,16 +3898,16 @@
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H96" s="0" t="n">
         <v>3</v>
@@ -3913,24 +3922,24 @@
         <v>100</v>
       </c>
       <c r="M96" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="N96" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H97" s="0" t="n">
         <v>3</v>
@@ -3945,15 +3954,15 @@
         <v>100</v>
       </c>
       <c r="M97" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="N97" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="F98" s="0" t="s">
         <v>17</v>
@@ -3970,16 +3979,16 @@
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H99" s="0" t="n">
         <v>2</v>
@@ -3994,24 +4003,24 @@
         <v>100</v>
       </c>
       <c r="M99" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="N99" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H100" s="0" t="n">
         <v>1</v>
@@ -4026,24 +4035,24 @@
         <v>100</v>
       </c>
       <c r="M100" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="N100" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H101" s="0" t="n">
         <v>3</v>
@@ -4058,15 +4067,15 @@
         <v>100</v>
       </c>
       <c r="M101" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="N101" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="F102" s="0" t="s">
         <v>17</v>
@@ -4083,16 +4092,16 @@
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H103" s="0" t="n">
         <v>3</v>
@@ -4107,24 +4116,24 @@
         <v>100</v>
       </c>
       <c r="M103" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="N103" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="G104" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H104" s="0" t="n">
         <v>2</v>
@@ -4139,24 +4148,24 @@
         <v>100</v>
       </c>
       <c r="M104" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="N104" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="G105" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H105" s="0" t="n">
         <v>1</v>
@@ -4171,24 +4180,24 @@
         <v>100</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="N105" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="G106" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H106" s="0" t="n">
         <v>1</v>
@@ -4203,15 +4212,15 @@
         <v>100</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="N106" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F107" s="0" t="s">
         <v>17</v>
@@ -4228,7 +4237,7 @@
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="F108" s="0" t="s">
         <v>17</v>
@@ -4245,16 +4254,16 @@
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H109" s="0" t="n">
         <v>2</v>
@@ -4277,16 +4286,16 @@
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B110" s="0" t="s">
         <v>322</v>
       </c>
-      <c r="B110" s="0" t="s">
-        <v>320</v>
-      </c>
       <c r="D110" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="G110" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H110" s="0" t="n">
         <v>2</v>
@@ -4309,16 +4318,16 @@
     </row>
     <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="G111" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H111" s="0" t="n">
         <v>2</v>
@@ -4341,16 +4350,16 @@
     </row>
     <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="G112" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H112" s="0" t="n">
         <v>2</v>
@@ -4373,16 +4382,16 @@
     </row>
     <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="G113" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H113" s="0" t="n">
         <v>2</v>
@@ -4405,16 +4414,16 @@
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G114" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H114" s="0" t="n">
         <v>2</v>
@@ -4437,16 +4446,16 @@
     </row>
     <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="G115" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H115" s="0" t="n">
         <v>1</v>
@@ -4469,16 +4478,16 @@
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="G116" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H116" s="0" t="n">
         <v>1</v>
@@ -4493,10 +4502,10 @@
         <v>100</v>
       </c>
       <c r="M116" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="N116" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>